<commit_message>
update v2 [new interface]
</commit_message>
<xml_diff>
--- a/data/processing/data_sigla.xlsx
+++ b/data/processing/data_sigla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BASELINE_SIGLA" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Controle" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="BASELINE_SIGLA" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Controle" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9 x BACKUP 8GB RAM 8vCPU (WEBSERVER)</t>
+          <t>9 x BACKUP 16GB RAM 8vCPU (WEBSERVER)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -865,6 +865,7 @@
           <t>9</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>Always On</t>
@@ -885,6 +886,8 @@
           <t>320</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>6x Daily</t>
@@ -904,7 +907,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4 x BACKUP 16GB RAM 16vCPU (WEBSERVER)</t>
+          <t>4 x BACKUP 32GB RAM 16vCPU (WEBSERVER)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -957,6 +960,8 @@
           <t>230</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>2x Daily</t>
@@ -1004,6 +1009,7 @@
           <t>3</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>Always On</t>
@@ -1024,6 +1030,8 @@
           <t>430</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>6x Daily</t>
@@ -1043,7 +1051,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3 x BACKUP 24GB RAM 8vCPU (WEBSERVER)</t>
+          <t>3 x BACKUP 32GB RAM 8vCPU (WEBSERVER)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1071,6 +1079,7 @@
           <t>3</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>Always On</t>
@@ -1091,6 +1100,8 @@
           <t>800</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>6x Daily</t>

</xml_diff>

<commit_message>
update v3 [new interface]
</commit_message>
<xml_diff>
--- a/data/processing/data_sigla.xlsx
+++ b/data/processing/data_sigla.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,250 +479,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MA0283</t>
+          <t>MA0278</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Homologation</t>
+          <t>Production</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BACKUP 16GB RAM 16vCPU (WEBSERVER)</t>
+          <t>APLICACOES 32GB RAM 8vCPU (APLICACOES)</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>230</v>
+        <v>430</v>
       </c>
       <c r="E2" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>WEBSERVER</t>
+          <t>APLICACOES</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>MA0284</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>BACKUP 16GB RAM 16vCPU (WEBSERVER)</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>230</v>
-      </c>
-      <c r="E3" t="n">
-        <v>16</v>
-      </c>
-      <c r="F3" t="n">
-        <v>16</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>WEBSERVER</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MA0285</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>BACKUP 16GB RAM 16vCPU (WEBSERVER)</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>170</v>
-      </c>
-      <c r="E4" t="n">
-        <v>16</v>
-      </c>
-      <c r="F4" t="n">
-        <v>16</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>WEBSERVER</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>MA0286</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>BACKUP 8GB RAM 4vCPU (WEBSERVER)</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>170</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>WEBSERVER</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MA0287</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BACKUP 16GB RAM 4vCPU (BACKUP)</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>230</v>
-      </c>
-      <c r="E6" t="n">
-        <v>16</v>
-      </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>BACKUP</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>MA0288</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>BACKUP 16GB RAM 8vCPU (BACKUP)</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>170</v>
-      </c>
-      <c r="E7" t="n">
-        <v>16</v>
-      </c>
-      <c r="F7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>BACKUP</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>MA0289</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BACKUP 8GB RAM 8vCPU (BACKUP)</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>230</v>
-      </c>
-      <c r="E8" t="n">
-        <v>8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>BACKUP</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>Windows Server</t>
         </is>
@@ -739,7 +523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -832,12 +616,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Production</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4 x BACKUP 16GB RAM 8vCPU (BACKUP)</t>
+          <t>3 x APLICACOES 32GB RAM 8vCPU (APLICACOES)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -852,7 +636,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>c6i.2xlarge</t>
+          <t>m6id.2xlarge</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -862,22 +646,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Hours/Week</t>
+          <t>Always On</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>On-Demand</t>
+          <t>1 Yr No Upfront EC2 Instance Savings Plan</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -887,241 +667,19 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>430</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2x Daily</t>
+          <t>6x Daily</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>6 x BACKUP 32GB RAM 16vCPU (WEBSERVER)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sa-east-1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>c6a.4xlarge</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Shared Instances</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Hours/Week</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>On-Demand</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>General Purpose SSD (gp3)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>230</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>2x Daily</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2 x BACKUP 8GB RAM 4vCPU (WEBSERVER)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>sa-east-1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>c6in.xlarge</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Shared Instances</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Hours/Week</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>On-Demand</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>General Purpose SSD (gp3)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>2x Daily</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Homologation</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2 x BACKUP 16GB RAM 4vCPU (BACKUP)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>sa-east-1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Windows Server</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>m6id.xlarge</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Shared Instances</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Hours/Week</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>On-Demand</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>General Purpose SSD (gp3)</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>230</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2x Daily</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
     </row>

</xml_diff>